<commit_message>
Ik doe maar eens een commit omdat dat tof is.
</commit_message>
<xml_diff>
--- a/Reservoirdogs/uren.xlsx
+++ b/Reservoirdogs/uren.xlsx
@@ -18,9 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>Mr. Black</t>
-  </si>
-  <si>
     <t>Mr. White</t>
   </si>
   <si>
@@ -33,9 +30,6 @@
     <t>RekenJezelfRijk.nl</t>
   </si>
   <si>
-    <t>Uren Mr. Black</t>
-  </si>
-  <si>
     <t>Uren Mr. White</t>
   </si>
   <si>
@@ -46,6 +40,12 @@
   </si>
   <si>
     <t>Uren resterend</t>
+  </si>
+  <si>
+    <t>Uren Mr. Pink</t>
+  </si>
+  <si>
+    <t>Mr. Pink</t>
   </si>
 </sst>
 </file>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O10"/>
+  <dimension ref="B2:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,28 +431,28 @@
   <sheetData>
     <row r="2" spans="2:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="3"/>
       <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F2" s="3"/>
       <c r="H2" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="L3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
@@ -460,14 +460,15 @@
         <v>41048</v>
       </c>
       <c r="C4" s="4">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1">
         <v>41048</v>
       </c>
       <c r="F4" s="4">
-        <v>7</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
@@ -476,16 +477,20 @@
       <c r="C5" s="4">
         <v>2</v>
       </c>
+      <c r="E5" s="1">
+        <v>41057</v>
+      </c>
+      <c r="H5" s="1"/>
       <c r="L5" t="s">
         <v>0</v>
       </c>
       <c r="M5">
         <f>SUM(C:C)</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="O5">
         <f>M5*25</f>
-        <v>275</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
@@ -495,35 +500,190 @@
       <c r="C6" s="4">
         <v>2</v>
       </c>
+      <c r="E6" s="1"/>
+      <c r="H6" s="1"/>
       <c r="L6" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="M6">
         <f>SUM(F:F)</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O6">
         <f>M6*25</f>
-        <v>175</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="H7" s="1"/>
       <c r="L7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M7">
         <f>SUM(I:I)</f>
         <v>0</v>
       </c>
     </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="H10" s="1"/>
       <c r="L10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M10">
         <f>120-M5-M6-M7</f>
-        <v>102</v>
-      </c>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Uren bijgewerkt, gimme peso's!
</commit_message>
<xml_diff>
--- a/Reservoirdogs/uren.xlsx
+++ b/Reservoirdogs/uren.xlsx
@@ -408,7 +408,7 @@
   <dimension ref="B2:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,6 +480,9 @@
       <c r="E5" s="1">
         <v>41057</v>
       </c>
+      <c r="F5" s="4">
+        <v>7</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="L5" t="s">
         <v>0</v>
@@ -507,11 +510,11 @@
       </c>
       <c r="M6">
         <f>SUM(F:F)</f>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="O6">
         <f>M6*25</f>
-        <v>125</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
@@ -545,7 +548,7 @@
       </c>
       <c r="M10">
         <f>120-M5-M6-M7</f>
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Loginshizzle toegevoegd, woei! Uurtjes bijgewerkt.
</commit_message>
<xml_diff>
--- a/Reservoirdogs/uren.xlsx
+++ b/Reservoirdogs/uren.xlsx
@@ -408,7 +408,7 @@
   <dimension ref="B2:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,11 +489,11 @@
       </c>
       <c r="M5">
         <f>SUM(C:C)</f>
-        <v>16</v>
+        <v>22.5</v>
       </c>
       <c r="O5">
         <f>M5*25</f>
-        <v>400</v>
+        <v>562.5</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
@@ -503,18 +503,23 @@
       <c r="C6" s="4">
         <v>2</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1">
+        <v>41062</v>
+      </c>
+      <c r="F6" s="4">
+        <v>6.5</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="L6" t="s">
         <v>9</v>
       </c>
       <c r="M6">
         <f>SUM(F:F)</f>
-        <v>12</v>
+        <v>20.5</v>
       </c>
       <c r="O6">
         <f>M6*25</f>
-        <v>300</v>
+        <v>512.5</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
@@ -524,7 +529,12 @@
       <c r="C7" s="4">
         <v>7</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1">
+        <v>41063</v>
+      </c>
+      <c r="F7" s="4">
+        <v>2</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="L7" t="s">
         <v>1</v>
@@ -535,7 +545,12 @@
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
+      <c r="B8" s="1">
+        <v>41062</v>
+      </c>
+      <c r="C8" s="4">
+        <v>6.5</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="H8" s="1"/>
     </row>
@@ -553,7 +568,7 @@
       </c>
       <c r="M10">
         <f>120-M5-M6-M7</f>
-        <v>92</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Begin gemaakt met kennisgroeppagina, MembersList toegevoegd.
</commit_message>
<xml_diff>
--- a/Reservoirdogs/uren.xlsx
+++ b/Reservoirdogs/uren.xlsx
@@ -408,7 +408,7 @@
   <dimension ref="B2:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,11 +515,11 @@
       </c>
       <c r="M6">
         <f>SUM(F:F)</f>
-        <v>20.5</v>
+        <v>22.5</v>
       </c>
       <c r="O6">
         <f>M6*25</f>
-        <v>512.5</v>
+        <v>562.5</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
@@ -533,7 +533,7 @@
         <v>41063</v>
       </c>
       <c r="F7" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H7" s="1"/>
       <c r="L7" t="s">
@@ -568,7 +568,7 @@
       </c>
       <c r="M10">
         <f>120-M5-M6-M7</f>
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Kleine tweakjes aan membergroup.
</commit_message>
<xml_diff>
--- a/Reservoirdogs/uren.xlsx
+++ b/Reservoirdogs/uren.xlsx
@@ -408,7 +408,7 @@
   <dimension ref="B2:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,11 +515,11 @@
       </c>
       <c r="M6">
         <f>SUM(F:F)</f>
-        <v>27.5</v>
+        <v>28</v>
       </c>
       <c r="O6">
         <f>M6*25</f>
-        <v>687.5</v>
+        <v>700</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
@@ -566,7 +566,12 @@
       <c r="C9" s="4">
         <v>5</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1">
+        <v>41061</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.5</v>
+      </c>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
@@ -578,7 +583,7 @@
       </c>
       <c r="M10">
         <f>120-M5-M6-M7</f>
-        <v>65</v>
+        <v>64.5</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Discussie met posts afgemaakt, enige wat nog moet is edit post.
</commit_message>
<xml_diff>
--- a/Reservoirdogs/uren.xlsx
+++ b/Reservoirdogs/uren.xlsx
@@ -408,7 +408,7 @@
   <dimension ref="B2:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,11 +515,11 @@
       </c>
       <c r="M6">
         <f>SUM(F:F)</f>
-        <v>38</v>
+        <v>39.5</v>
       </c>
       <c r="O6">
         <f>M6*25</f>
-        <v>950</v>
+        <v>987.5</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
@@ -593,7 +593,7 @@
       </c>
       <c r="M10">
         <f>120-M5-M6-M7</f>
-        <v>36.5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
@@ -607,7 +607,7 @@
         <v>41091</v>
       </c>
       <c r="F11" s="4">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="H11" s="1"/>
     </row>

</xml_diff>

<commit_message>
changelog gewijzigd, uren aangepast.
</commit_message>
<xml_diff>
--- a/Reservoirdogs/uren.xlsx
+++ b/Reservoirdogs/uren.xlsx
@@ -408,7 +408,7 @@
   <dimension ref="B2:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,11 +515,11 @@
       </c>
       <c r="M6">
         <f>SUM(F:F)</f>
-        <v>41</v>
+        <v>41.5</v>
       </c>
       <c r="O6">
         <f>M6*25</f>
-        <v>1025</v>
+        <v>1037.5</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
@@ -593,7 +593,7 @@
       </c>
       <c r="M10">
         <f>120-M5-M6-M7</f>
-        <v>30.5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
@@ -622,7 +622,7 @@
         <v>41095</v>
       </c>
       <c r="F12" s="4">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="H12" s="1"/>
     </row>

</xml_diff>

<commit_message>
Profielpagina gestijld, notities gestijld.
</commit_message>
<xml_diff>
--- a/Reservoirdogs/uren.xlsx
+++ b/Reservoirdogs/uren.xlsx
@@ -408,7 +408,7 @@
   <dimension ref="B2:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,11 +515,11 @@
       </c>
       <c r="M6">
         <f>SUM(F:F)</f>
-        <v>41.5</v>
+        <v>43</v>
       </c>
       <c r="O6">
         <f>M6*25</f>
-        <v>1037.5</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
@@ -593,7 +593,7 @@
       </c>
       <c r="M10">
         <f>120-M5-M6-M7</f>
-        <v>28</v>
+        <v>26.5</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
@@ -633,7 +633,12 @@
       <c r="C13" s="4">
         <v>6</v>
       </c>
-      <c r="E13" s="1"/>
+      <c r="E13" s="1">
+        <v>41098</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1.5</v>
+      </c>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Styling toegevoegd voor quotes. Een quote van een quote is nog steeds kut. Maarja, tis niet anders.
</commit_message>
<xml_diff>
--- a/Reservoirdogs/uren.xlsx
+++ b/Reservoirdogs/uren.xlsx
@@ -408,7 +408,7 @@
   <dimension ref="B2:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,11 +515,11 @@
       </c>
       <c r="M6">
         <f>SUM(F:F)</f>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O6">
         <f>M6*25</f>
-        <v>1075</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
@@ -593,7 +593,7 @@
       </c>
       <c r="M10">
         <f>120-M5-M6-M7</f>
-        <v>24.5</v>
+        <v>23.5</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
@@ -648,7 +648,12 @@
       <c r="C14" s="4">
         <v>2.5</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1">
+        <v>41100</v>
+      </c>
+      <c r="F14" s="4">
+        <v>1</v>
+      </c>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Landstede skin er grotendeels in geramd.
</commit_message>
<xml_diff>
--- a/Reservoirdogs/uren.xlsx
+++ b/Reservoirdogs/uren.xlsx
@@ -408,7 +408,7 @@
   <dimension ref="B2:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,11 +515,11 @@
       </c>
       <c r="M6">
         <f>SUM(F:F)</f>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="O6">
         <f>M6*25</f>
-        <v>1100</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
@@ -593,7 +593,7 @@
       </c>
       <c r="M10">
         <f>120-M5-M6-M7</f>
-        <v>17.5</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
@@ -663,7 +663,12 @@
       <c r="C15" s="4">
         <v>2</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1">
+        <v>41161</v>
+      </c>
+      <c r="F15" s="4">
+        <v>2</v>
+      </c>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Alle projecten en alle kennisgroepen toegevoegd aan mijn projecten en mijn kennisgroepen, juiste font toegevoegd.
</commit_message>
<xml_diff>
--- a/Reservoirdogs/uren.xlsx
+++ b/Reservoirdogs/uren.xlsx
@@ -408,7 +408,7 @@
   <dimension ref="B2:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,11 +515,11 @@
       </c>
       <c r="M6">
         <f>SUM(F:F)</f>
-        <v>46</v>
+        <v>47.5</v>
       </c>
       <c r="O6">
         <f>M6*25</f>
-        <v>1150</v>
+        <v>1187.5</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
@@ -593,7 +593,7 @@
       </c>
       <c r="M10">
         <f>120-M5-M6-M7</f>
-        <v>11.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
@@ -678,7 +678,12 @@
       <c r="C16" s="4">
         <v>4</v>
       </c>
-      <c r="E16" s="1"/>
+      <c r="E16" s="1">
+        <v>41166</v>
+      </c>
+      <c r="F16" s="4">
+        <v>1.5</v>
+      </c>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Documentenverdieping gefikst, wat layout dingetjes gefikst.
</commit_message>
<xml_diff>
--- a/Reservoirdogs/uren.xlsx
+++ b/Reservoirdogs/uren.xlsx
@@ -408,7 +408,7 @@
   <dimension ref="B2:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,11 +515,11 @@
       </c>
       <c r="M6">
         <f>SUM(F:F)</f>
-        <v>47.5</v>
+        <v>49.5</v>
       </c>
       <c r="O6">
         <f>M6*25</f>
-        <v>1187.5</v>
+        <v>1237.5</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
@@ -593,7 +593,7 @@
       </c>
       <c r="M10">
         <f>120-M5-M6-M7</f>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
@@ -693,7 +693,12 @@
       <c r="C17" s="4">
         <v>2</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E17" s="1">
+        <v>41167</v>
+      </c>
+      <c r="F17" s="4">
+        <v>2</v>
+      </c>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Populaire projecten toegevoegd, media embed meuk. Joepie!
</commit_message>
<xml_diff>
--- a/Reservoirdogs/uren.xlsx
+++ b/Reservoirdogs/uren.xlsx
@@ -408,7 +408,7 @@
   <dimension ref="B2:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,11 +489,11 @@
       </c>
       <c r="M5">
         <f>SUM(C:C)</f>
-        <v>62.5</v>
+        <v>69.5</v>
       </c>
       <c r="O5">
         <f>M5*25</f>
-        <v>1562.5</v>
+        <v>1737.5</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
@@ -515,11 +515,11 @@
       </c>
       <c r="M6">
         <f>SUM(F:F)</f>
-        <v>49.5</v>
+        <v>58.5</v>
       </c>
       <c r="O6">
         <f>M6*25</f>
-        <v>1237.5</v>
+        <v>1462.5</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
@@ -593,7 +593,7 @@
       </c>
       <c r="M10">
         <f>120-M5-M6-M7</f>
-        <v>8</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
@@ -708,7 +708,12 @@
       <c r="C18" s="4">
         <v>1</v>
       </c>
-      <c r="E18" s="1"/>
+      <c r="E18" s="1">
+        <v>41175</v>
+      </c>
+      <c r="F18" s="4">
+        <v>7</v>
+      </c>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -718,7 +723,12 @@
       <c r="C19" s="4">
         <v>2</v>
       </c>
-      <c r="E19" s="1"/>
+      <c r="E19" s="1">
+        <v>41193</v>
+      </c>
+      <c r="F19" s="4">
+        <v>2</v>
+      </c>
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -762,7 +772,12 @@
       <c r="H23" s="1"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
+      <c r="B24" s="1">
+        <v>41175</v>
+      </c>
+      <c r="C24" s="4">
+        <v>7</v>
+      </c>
       <c r="E24" s="1"/>
       <c r="H24" s="1"/>
     </row>

</xml_diff>